<commit_message>
Test-4 (this year input)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/tests/test-4.xlsx
+++ b/migforecasting/less100/tests/test-4.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="ThisYear" sheetId="1" r:id="rId1"/>
+    <sheet name="NextYear" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,14 +19,58 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+  <si>
+    <t>Random Forest-100 (citiesdataset-Dcor-4.csv) - next year, without dollar</t>
+  </si>
+  <si>
+    <t>test input (MAPE)</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Old input</t>
+  </si>
+  <si>
+    <t>Input60</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-Dcor-4.csv) - next year, without dollar, здравохранения, квартир, фондов и предприятий</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,11 +94,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +167,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +207,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -331,9 +389,892 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:K58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.1481210605466057</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>5.5255428545068126</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13.85994804453242</v>
+      </c>
+      <c r="J7" s="2">
+        <f>J6+1</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>8.4812690371302804</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>14.69774262508931</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8:J55" si="1">J7+1</f>
+        <v>3</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9.6399431328745386</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>13.534942106117629</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4.1909421853909619</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>13.59123562106064</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>8.9864538547049122</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>13.0628911445291</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
+        <v>8.8086066089528714</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5.3450509632131133</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>6.8591751950739042</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>13.40164592170431</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="3">
+        <v>7.1072733297194493</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10.49650927075284</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K14" s="3">
+        <v>8.7774154873708454</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>14.96009619585775</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K15" s="3">
+        <v>7.8425956621343618</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10.58298944690169</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K16" s="3">
+        <v>7.9658733430382416</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>16.572055498155368</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K17" s="3">
+        <v>7.6698551838365088</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10.068455035771089</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K18" s="3">
+        <v>7.3055599836547147</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>15.095852125560061</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="K19" s="3">
+        <v>8.7059713546853779</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>14.580532115294931</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="K20" s="3">
+        <v>9.5423257420114815</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>13.594522798108059</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K21" s="3">
+        <v>7.81636726123706</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>12.19523209925158</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K22" s="3">
+        <v>6.334071609133467</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>7.5687056569431732</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="K23" s="3">
+        <v>6.1818493806782282</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>11.826297189771889</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K24" s="3">
+        <v>8.9151675512011739</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>20.979144368651809</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10.28595546453278</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>6.6869997184492256</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="K26" s="3">
+        <v>8.5169738117672456</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>12.6741228221226</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="K27" s="3">
+        <v>5.9959882973966891</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>14.473228843935541</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="K28" s="3">
+        <v>6.2413798055835317</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5.671760382146469</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="K29" s="3">
+        <v>9.539441283655524</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>18.158375409760279</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="K30" s="3">
+        <v>7.6497904510869379</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>13.141445055348109</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="K31" s="3">
+        <v>9.370843677352763</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>13.346927645623801</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="K32" s="3">
+        <v>10.02224585915507</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>16.188037804052939</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K33" s="3">
+        <v>7.7368967836498772</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>12.95175101188851</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="K34" s="3">
+        <v>10.320781145810059</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>13.855968371133759</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K35" s="3">
+        <v>7.6194116600115338</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>10.005451344738191</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K36" s="3">
+        <v>8.8011915926335789</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>13.900603759205341</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K37" s="3">
+        <v>7.4011454616565908</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>11.83244859385184</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K38" s="3">
+        <v>8.2943591175278915</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>15.07161662992092</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K39" s="3">
+        <v>8.2588524379497201</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>9.7514383208474786</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="K40" s="3">
+        <v>6.1444545463703353</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>7.1759526938350966</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="K41" s="3">
+        <v>7.9991131756370821</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>15.374485602035829</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="K42" s="3">
+        <v>8.6709620902330329</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>13.820234635034559</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K43" s="3">
+        <v>7.2982508772931283</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>15.24218224773244</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="K44" s="3">
+        <v>9.4864530878054403</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>16.678039794780791</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K45" s="3">
+        <v>6.3003220779227158</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>10.88595419114036</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="K46" s="3">
+        <v>7.4922137393950186</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>8.176823114886588</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="K47" s="3">
+        <v>6.0802827766057268</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>6.1285308034506896</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="K48" s="3">
+        <v>8.3403621614661105</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>8.4374582739136699</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K49" s="3">
+        <v>9.9966564264081317</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>17.46714983719237</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K50" s="3">
+        <v>8.5367706226991569</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>12.02035334191277</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="K51" s="3">
+        <v>9.7371735401117707</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>10.042343746622301</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="K52" s="3">
+        <v>7.5075155449844724</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>11.22729204082408</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="K53" s="3">
+        <v>6.0111245512190452</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>5.9984896735634372</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="K54" s="3">
+        <v>8.8741432612013789</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>9.5490284786513442</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K55" s="3">
+        <v>5.9835221294288106</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AVERAGE(D6:D55)</f>
+        <v>12.161929269528295</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K57" s="3">
+        <f>AVERAGE(K6:K55)</f>
+        <v>7.9434167243177276</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="3">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>3.5638395057567669</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K58" s="3">
+        <f>_xlfn.STDEV.S(K6:K55)</f>
+        <v>1.3986178872752852</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Prep for classification & plot4test
</commit_message>
<xml_diff>
--- a/migforecasting/less100/tests/test-4.xlsx
+++ b/migforecasting/less100/tests/test-4.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="ThisYear and NextYear" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -129,6 +132,1124 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" b="1"/>
+              <a:t>Прогноз миграции на малых городах РФ (ЛО</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" b="1" baseline="0"/>
+              <a:t> И РО)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" b="1"/>
+              <a:t>Среднее отклонение по </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>MAPE</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]NextYear and ThisYear'!$E$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]NextYear and ThisYear'!$F$62:$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Next Year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>This Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('ThisYear and NextYear'!$AC$57,'ThisYear and NextYear'!$K$57)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.004877967075954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9434167243177276</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD83-4DD4-874D-CC9C7A6E0A67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]NextYear and ThisYear'!$E$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]NextYear and ThisYear'!$F$62:$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Next Year</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>This Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('ThisYear and NextYear'!$AC$58,'ThisYear and NextYear'!$K$58)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0312948556882169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3986178872752852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CD83-4DD4-874D-CC9C7A6E0A67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="1209861695"/>
+        <c:axId val="1209860863"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1209861695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1209860863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1209860863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1209861695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>530679</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>570139</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>36739</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Диаграмма 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="NextYear and ThisYear"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="62">
+          <cell r="F62" t="str">
+            <v>Next Year</v>
+          </cell>
+          <cell r="G62" t="str">
+            <v>This Year</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="E63" t="str">
+            <v>Avg</v>
+          </cell>
+          <cell r="F63">
+            <v>9.2185059697096214</v>
+          </cell>
+          <cell r="G63">
+            <v>12.161929269528295</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="E64" t="str">
+            <v>SD</v>
+          </cell>
+          <cell r="F64">
+            <v>3.5467676138490525</v>
+          </cell>
+          <cell r="G64">
+            <v>3.5638395057567669</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AC58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE38" sqref="AE38"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y73" sqref="Y73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,5 +3139,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hybrid model (KZ) for any input
</commit_message>
<xml_diff>
--- a/migforecasting/less100/tests/test-4.xlsx
+++ b/migforecasting/less100/tests/test-4.xlsx
@@ -1228,22 +1228,10 @@
           <cell r="E63" t="str">
             <v>Avg</v>
           </cell>
-          <cell r="F63">
-            <v>9.2185059697096214</v>
-          </cell>
-          <cell r="G63">
-            <v>12.161929269528295</v>
-          </cell>
         </row>
         <row r="64">
           <cell r="E64" t="str">
             <v>SD</v>
-          </cell>
-          <cell r="F64">
-            <v>3.5467676138490525</v>
-          </cell>
-          <cell r="G64">
-            <v>3.5638395057567669</v>
           </cell>
         </row>
       </sheetData>
@@ -1517,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AC58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y73" sqref="Y73"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:29" x14ac:dyDescent="0.25">

</xml_diff>